<commit_message>
Arreglo el crud y tablas
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,60 +441,50 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>dia</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>dia</t>
+          <t>mes</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>unidad_numero</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>mes</t>
+          <t>clase_numero</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>unidad_numero</t>
+          <t>curso</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>clase_numero</t>
+          <t>caracter_clase</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>curso</t>
+          <t>contenidos_tematicos</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>caracter_clase</t>
+          <t>actividades</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>contenidos_tematicos</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>actividades</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>observaciones</t>
         </is>
@@ -506,22 +496,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PEPE</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>25</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>5b</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>aaaaa</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nnnnnn</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>sssss</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>ccccc</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -529,123 +551,52 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MARINA</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>30</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>jesucita</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>18</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>sadfasd</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>24</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>2024-09-07</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>09</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>6a</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>sadfa</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>asdfas</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>fsafasd</t>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5b</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>asdfa</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>sda</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>fda</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduzco estilos para proximos cambios
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,37 +496,31 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-09-07</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+          <t>2024-09-08</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>5b</t>
+          <t>6a</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>aaaaa</t>
+          <t>GSDFGSDGDSFGD</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -551,52 +545,315 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>5aaa</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5b</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>asdfa</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>sda</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BBBB</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-09-07</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>32</v>
+      </c>
+      <c r="E4" t="n">
+        <v>23</v>
+      </c>
+      <c r="F4" t="n">
+        <v>23</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6a</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>fasd</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hola te amo mucho</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-09-08</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2024-09-07</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>5b</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Dhjfnsjfj</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ndjfjdndjfjd</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Djfjdjtjdj</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Jfjfjfjdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>fasdf</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>43434</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>6a</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>sdgsdfg</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>sdfgsd</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>fgsdfgsdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>asdfasd</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>223223-02-23</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>as2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>5b</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>asdfa</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>sdf</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>sda</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>fda</t>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>232</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>6a</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>sadfsa</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>dfasd</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>fasdf</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>asf</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>zzzz</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-09-08</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>6a</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>sdaf</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>sdfas</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>df</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
primer commit de esta rama
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,11 +492,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>Hola te amo mucho</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -504,112 +504,120 @@
           <t>2024-09-08</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
-        <v>6</v>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6a</t>
+          <t>M1B</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>GSDFGSDGDSFGD</t>
+          <t>Práctica</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>nnnnnn</t>
+          <t>Ndjfjdndjfjd</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>sssss</t>
+          <t>Djfjdjtjdj</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>ccccc</t>
+          <t>Jfjfjfjdd</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5aaa</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-09-07</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>23</v>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>fasdf</t>
+        </is>
       </c>
       <c r="E3" t="n">
         <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>43434</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5b</t>
+          <t>6a</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>asdfa</t>
+          <t>sdgsdfg</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>sdf</t>
+          <t>dfg</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>sda</t>
+          <t>sdfgsd</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>fda</t>
+          <t>fgsdfgsdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BBBB</t>
+          <t>asdfasd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-09-07</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>32</v>
+          <t>223223-02-23</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>as2</t>
+        </is>
       </c>
       <c r="E4" t="n">
         <v>23</v>
       </c>
       <c r="F4" t="n">
-        <v>23</v>
+        <v>232</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -618,32 +626,32 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>sadfsa</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>dfasd</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>fasdf</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>fasd</t>
+          <t>asf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hola te amo mucho</t>
+          <t>AAAAAAAAAAA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -653,14 +661,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2423423</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>23423423</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>34243</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -669,179 +677,210 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dhjfnsjfj</t>
+          <t>ERWER</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Ndjfjdndjfjd</t>
+          <t>FDSFASDF</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Djfjdjtjdj</t>
+          <t>FDSFDS</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Jfjfjfjdd</t>
+          <t>FDSFSFDSF</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-09-13</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>fasdf</t>
-        </is>
-      </c>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F6" t="n">
-        <v>43434</v>
+        <v>23</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>6a</t>
+          <t>M1B</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>sdgsdfg</t>
+          <t>ASDF</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>dfg</t>
+          <t>ASFASDF</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>sdfgsd</t>
+          <t>ASDFAS</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>fgsdfgsdf</t>
+          <t>DFA</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>asdfasd</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>223223-02-23</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>as2</t>
-        </is>
-      </c>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>23</v>
+        <v>232</v>
       </c>
       <c r="F7" t="n">
         <v>232</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>6a</t>
+          <t>S6A</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>sadfsa</t>
+          <t>Práctica</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>dfasd</t>
+          <t>sdfa</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>fasdf</t>
+          <t>sdfas</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>asf</t>
+          <t>dfas</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AAAAAAAAAAA</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-09-08</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2423423</t>
-        </is>
-      </c>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>23423423</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>34243</t>
-        </is>
-      </c>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>6a</t>
+          <t>M1B</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ERWER</t>
+          <t>Teórico/Práctica</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>FDSFASDF</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>FDSFDS</t>
+          <t>asdfsa</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>FDSFSFDSF</t>
+          <t>dfsaddf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>TM</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Explicación</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>safd</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>asdfas</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
anda el responsive, la funcionalidad y estilos ok. Proximo paso merge y buscar mas estilos y conectar con sheets
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,10 +509,8 @@
           <t>2</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="E2" t="n">
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
@@ -651,12 +649,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AAAAAAAAAAA</t>
+          <t>miernesssss</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-09-08</t>
+          <t>2024-09-13</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -665,34 +663,34 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>23423423</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>34243</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>6a</t>
+          <t>S6A</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ERWER</t>
+          <t>Práctica</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>FDSFASDF</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>FDSFDS</t>
+          <t>sadf</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>FDSFSFDSF</t>
+          <t>asdf</t>
         </is>
       </c>
     </row>
@@ -792,11 +790,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>234</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -805,45 +803,43 @@
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="E8" t="n">
+        <v>23</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>M1B</t>
+          <t>M1A</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Teórico/Práctica</t>
+          <t>Explicación</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
+          <t>safd</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
           <t>asdf</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>asdfsa</t>
-        </is>
-      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>dfsaddf</t>
+          <t>asdfas</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -852,35 +848,125 @@
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="E9" t="n">
+        <v>5</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
+          <t>M1A</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Explicación</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Jfjdjd</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Fjfjdjf</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Jfnfjjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>miernes</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>S6A</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Práctica</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>sadf</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BNBBB</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>3232</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>TM</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Explicación</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>safd</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Examen</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>sadf</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>asdf</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>asdfas</t>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>asdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Funcionalidades y estilos casi completo. falta sheets
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,62 +645,58 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>miernesssss</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-09-13</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2423423</t>
-        </is>
-      </c>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F5" t="n">
-        <v>34243</v>
+        <v>23</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>S6A</t>
+          <t>M1B</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Práctica</t>
+          <t>ASDF</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>ASFASDF</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>sadf</t>
+          <t>ASDFAS</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>DFA</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>234</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -712,259 +708,75 @@
       <c r="E6" t="n">
         <v>23</v>
       </c>
-      <c r="F6" t="n">
-        <v>23</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>M1B</t>
+          <t>M1A</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ASDF</t>
+          <t>Explicación</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ASFASDF</t>
+          <t>safd</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ASDFAS</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>DFA</t>
+          <t>asdfas</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>HOLA MIBIDA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-09-12</t>
+          <t>2024-09-13</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>232</v>
-      </c>
-      <c r="F7" t="n">
-        <v>232</v>
-      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3232</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>S6A</t>
+          <t>TM</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Práctica</t>
+          <t>Teórico/Práctica</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>sdfa</t>
+          <t>sadf</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>sdfas</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
-        <is>
-          <t>dfas</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>11</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2024-09-12</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>23</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>M1A</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Explicación</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>safd</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>asdfas</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Jueves</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2024-09-12</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>M1A</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Explicación</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Jfjdjd</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Fjfjdjf</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Jfnfjjd</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>miernes</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2024-09-13</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>5</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>S6A</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Práctica</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>sadf</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>BNBBB</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2024-09-13</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>3232</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>TM</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Examen</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>sadf</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
         <is>
           <t>asdf</t>
         </is>

</xml_diff>